<commit_message>
Log in and transfer in functionality is done with dynamic code
</commit_message>
<xml_diff>
--- a/artifactid/files/LoginCred.xlsx
+++ b/artifactid/files/LoginCred.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">URL</t>
   </si>
@@ -34,7 +34,30 @@
     <t xml:space="preserve">Password</t>
   </si>
   <si>
-    <t xml:space="preserve">LocationSelection</t>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">medication</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> name</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">quantity</t>
   </si>
   <si>
     <t xml:space="preserve">https://hospital-staging.strongroom.ai/login</t>
@@ -47,6 +70,9 @@
   </si>
   <si>
     <t xml:space="preserve">stew-dazzling-washtub!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">guaifenesin 100 mg/5 mL oral liquid</t>
   </si>
 </sst>
 </file>
@@ -56,7 +82,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -82,11 +108,26 @@
       <u val="single"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Monospace"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Monospace"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
+      <u val="single"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -136,7 +177,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -145,8 +186,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -166,19 +215,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:AMJ2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -194,23 +243,34 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
+      <c r="A2" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AMI2" s="0"/>
+      <c r="AMJ2" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>